<commit_message>
Use floating rule for now
</commit_message>
<xml_diff>
--- a/resources/output.xlsx
+++ b/resources/output.xlsx
@@ -422,7 +422,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,20 +478,6 @@
         </is>
       </c>
     </row>
-    <row r="4" ht="30" customHeight="1">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>lan</t>
-        </is>
-      </c>
-      <c r="B4" s="2" t="inlineStr"/>
-      <c r="C4" s="2" t="inlineStr">
-        <is>
-          <t>Protocol : * - Port : *
-Protocol : * - Port : *</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Better support for 'any' protocol
</commit_message>
<xml_diff>
--- a/resources/output.xlsx
+++ b/resources/output.xlsx
@@ -422,7 +422,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -431,8 +431,10 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="20" customWidth="1" min="1" max="1"/>
-    <col width="34" customWidth="1" min="2" max="2"/>
-    <col width="23" customWidth="1" min="3" max="3"/>
+    <col width="23" customWidth="1" min="2" max="2"/>
+    <col width="27" customWidth="1" min="3" max="3"/>
+    <col width="27" customWidth="1" min="4" max="4"/>
+    <col width="27" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" customHeight="1">
@@ -443,38 +445,51 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>178.3.4.0/22</t>
+          <t>10.0.0.0/24</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>10.0.0.34/32</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>10.0.0.49/32</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>10.0.0.23/32</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="30" customHeight="1">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
           <t>*</t>
         </is>
       </c>
-    </row>
-    <row r="2" ht="15" customHeight="1">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>127.0.0.42/32</t>
-        </is>
-      </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>Protocol : TCP - Port : (53, 5060)</t>
-        </is>
-      </c>
-      <c r="C2" s="2" t="inlineStr"/>
-    </row>
-    <row r="3" ht="15" customHeight="1">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>*</t>
-        </is>
-      </c>
-      <c r="B3" s="2" t="inlineStr"/>
-      <c r="C3" s="2" t="inlineStr">
-        <is>
           <t>Protocol : * - Port : *</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>Protocol : TCP - Port : 80
+Protocol : TCP - Port : 443</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="inlineStr">
+        <is>
+          <t>Protocol : TCP - Port : 143
+Protocol : TCP - Port : 993</t>
+        </is>
+      </c>
+      <c r="E2" s="2" t="inlineStr">
+        <is>
+          <t>Protocol : UDP - Port : 389</t>
         </is>
       </c>
     </row>

</xml_diff>